<commit_message>
added new logic to many functions and recorrected.
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27c8b8992c89f3d2/Documents/quantinuum/task_2/latest_work/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104808F95F5A445BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64ED03CA-FAE1-41C6-A972-ACE1AC76C374}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC104808F95F5A445BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07FCEA65-D674-400D-B44F-EA3F559ED377}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+  <si>
+    <t>standard_user</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>error_user</t>
+  </si>
+  <si>
+    <t>visual_user</t>
+  </si>
+  <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>invalid_user</t>
+  </si>
+  <si>
+    <t>wrong_password</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Gabbar</t>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>ASDFGH</t>
+  </si>
   <si>
     <t>username</t>
   </si>
@@ -34,40 +76,16 @@
     <t>password</t>
   </si>
   <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Postal_code</t>
+  </si>
+  <si>
     <t>expected_result</t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>performance_glitch_user</t>
-  </si>
-  <si>
-    <t>error_user</t>
-  </si>
-  <si>
-    <t>visual_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>invalid_user</t>
-  </si>
-  <si>
-    <t>wrong_password</t>
-  </si>
-  <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>error</t>
   </si>
 </sst>
 </file>
@@ -385,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,93 +414,168 @@
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>13</v>
       </c>
     </row>
@@ -493,103 +586,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DDC065-66D2-42B7-9C25-027576DC2212}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>